<commit_message>
Made several updates and changes to the website.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravenskelton/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46565062-0B8E-A94A-A9E1-6AA68DDFA56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F92975D0-C59F-7F41-B4B1-EA37CF55D8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="27">
   <si>
     <t>Long</t>
   </si>
@@ -176,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +186,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
@@ -246,6 +252,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4051,7 +4062,7 @@
         <v>26.4</v>
       </c>
       <c r="I116">
-        <f>-F116-G116/60-H116/3600</f>
+        <f t="shared" ref="I116:I134" si="16">-F116-G116/60-H116/3600</f>
         <v>-90.407333333333341</v>
       </c>
     </row>
@@ -4069,7 +4080,7 @@
         <v>15.3</v>
       </c>
       <c r="E117" s="4">
-        <f>B117+C117/60+D117/3600</f>
+        <f t="shared" ref="E117:E134" si="17">B117+C117/60+D117/3600</f>
         <v>29.737583333333333</v>
       </c>
       <c r="F117" s="1">
@@ -4082,7 +4093,7 @@
         <v>50.4</v>
       </c>
       <c r="I117">
-        <f>-F117-G117/60-H117/3600</f>
+        <f t="shared" si="16"/>
         <v>-90.647333333333336</v>
       </c>
     </row>
@@ -4100,7 +4111,7 @@
         <v>48.4</v>
       </c>
       <c r="E118" s="4">
-        <f>B118+C118/60+D118/3600</f>
+        <f t="shared" si="17"/>
         <v>29.646777777777778</v>
       </c>
       <c r="F118" s="1">
@@ -4113,7 +4124,7 @@
         <v>27.4</v>
       </c>
       <c r="I118">
-        <f>-F118-G118/60-H118/3600</f>
+        <f t="shared" si="16"/>
         <v>-90.540944444444449</v>
       </c>
       <c r="L118" s="4"/>
@@ -4132,7 +4143,7 @@
         <v>0.3</v>
       </c>
       <c r="E119" s="4">
-        <f>B119+C119/60+D119/3600</f>
+        <f t="shared" si="17"/>
         <v>29.86675</v>
       </c>
       <c r="F119" s="1">
@@ -4145,7 +4156,7 @@
         <v>58.8</v>
       </c>
       <c r="I119">
-        <f>-F119-G119/60-H119/3600</f>
+        <f t="shared" si="16"/>
         <v>-90.599666666666664</v>
       </c>
     </row>
@@ -4163,7 +4174,7 @@
         <v>8.1359999999999992</v>
       </c>
       <c r="E120" s="4">
-        <f>B120+C120/60+D120/3600</f>
+        <f t="shared" si="17"/>
         <v>30.535593333333335</v>
       </c>
       <c r="F120" s="1">
@@ -4176,7 +4187,7 @@
         <v>22.564</v>
       </c>
       <c r="I120">
-        <f>-F120-G120/60-H120/3600</f>
+        <f t="shared" si="16"/>
         <v>-91.089601111111108</v>
       </c>
     </row>
@@ -4194,7 +4205,7 @@
         <v>2.2879999999999998</v>
       </c>
       <c r="E121" s="4">
-        <f>B121+C121/60+D121/3600</f>
+        <f t="shared" si="17"/>
         <v>30.533968888888889</v>
       </c>
       <c r="F121" s="1">
@@ -4207,7 +4218,7 @@
         <v>20.337</v>
       </c>
       <c r="I121">
-        <f>-F121-G121/60-H121/3600</f>
+        <f t="shared" si="16"/>
         <v>-91.0889825</v>
       </c>
     </row>
@@ -4225,7 +4236,7 @@
         <v>18.3</v>
       </c>
       <c r="E122" s="4">
-        <f>B122+C122/60+D122/3600</f>
+        <f t="shared" si="17"/>
         <v>32.271749999999997</v>
       </c>
       <c r="F122" s="1">
@@ -4238,7 +4249,7 @@
         <v>44.4</v>
       </c>
       <c r="I122">
-        <f>-F122-G122/60-H122/3600</f>
+        <f t="shared" si="16"/>
         <v>-93.512333333333331</v>
       </c>
     </row>
@@ -4256,7 +4267,7 @@
         <v>12.2</v>
       </c>
       <c r="E123" s="4">
-        <f>B123+C123/60+D123/3600</f>
+        <f t="shared" si="17"/>
         <v>32.336722222222228</v>
       </c>
       <c r="F123" s="1">
@@ -4269,7 +4280,7 @@
         <v>27.6</v>
       </c>
       <c r="I123">
-        <f>-F123-G123/60-H123/3600</f>
+        <f t="shared" si="16"/>
         <v>-93.741</v>
       </c>
     </row>
@@ -4287,7 +4298,7 @@
         <v>31.1</v>
       </c>
       <c r="E124" s="4">
-        <f>B124+C124/60+D124/3600</f>
+        <f t="shared" si="17"/>
         <v>32.491972222222223</v>
       </c>
       <c r="F124" s="1">
@@ -4300,7 +4311,7 @@
         <v>1.4</v>
       </c>
       <c r="I124">
-        <f>-F124-G124/60-H124/3600</f>
+        <f t="shared" si="16"/>
         <v>-93.850388888888887</v>
       </c>
     </row>
@@ -4318,7 +4329,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E125" s="4">
-        <f>B125+C125/60+D125/3600</f>
+        <f t="shared" si="17"/>
         <v>32.635750000000002</v>
       </c>
       <c r="F125" s="1">
@@ -4331,7 +4342,7 @@
         <v>30.8</v>
       </c>
       <c r="I125">
-        <f>-F125-G125/60-H125/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.6418888888889</v>
       </c>
     </row>
@@ -4349,7 +4360,7 @@
         <v>50.6</v>
       </c>
       <c r="E126" s="4">
-        <f>B126+C126/60+D126/3600</f>
+        <f t="shared" si="17"/>
         <v>32.680722222222222</v>
       </c>
       <c r="F126" s="1">
@@ -4362,7 +4373,7 @@
         <v>59.5</v>
       </c>
       <c r="I126">
-        <f>-F126-G126/60-H126/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.649861111111122</v>
       </c>
     </row>
@@ -4380,7 +4391,7 @@
         <v>26.9</v>
       </c>
       <c r="E127" s="4">
-        <f>B127+C127/60+D127/3600</f>
+        <f t="shared" si="17"/>
         <v>32.857472222222221</v>
       </c>
       <c r="F127" s="1">
@@ -4393,7 +4404,7 @@
         <v>32.200000000000003</v>
       </c>
       <c r="I127">
-        <f>-F127-G127/60-H127/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.575611111111101</v>
       </c>
     </row>
@@ -4411,7 +4422,7 @@
         <v>57.4</v>
       </c>
       <c r="E128" s="4">
-        <f>B128+C128/60+D128/3600</f>
+        <f t="shared" si="17"/>
         <v>32.782611111111109</v>
       </c>
       <c r="F128" s="1">
@@ -4424,7 +4435,7 @@
         <v>26.9</v>
       </c>
       <c r="I128">
-        <f>-F128-G128/60-H128/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.490805555555553</v>
       </c>
     </row>
@@ -4442,7 +4453,7 @@
         <v>47.7</v>
       </c>
       <c r="E129" s="4">
-        <f>B129+C129/60+D129/3600</f>
+        <f t="shared" si="17"/>
         <v>31.929916666666667</v>
       </c>
       <c r="F129" s="1">
@@ -4455,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="I129">
-        <f>-F129-G129/60-H129/3600</f>
+        <f t="shared" si="16"/>
         <v>-91.766944444444448</v>
       </c>
     </row>
@@ -4473,7 +4484,7 @@
         <v>42.6</v>
       </c>
       <c r="E130" s="4">
-        <f>B130+C130/60+D130/3600</f>
+        <f t="shared" si="17"/>
         <v>32.811833333333333</v>
       </c>
       <c r="F130" s="1">
@@ -4486,7 +4497,7 @@
         <v>32</v>
       </c>
       <c r="I130">
-        <f>-F130-G130/60-H130/3600</f>
+        <f t="shared" si="16"/>
         <v>-91.192222222222227</v>
       </c>
     </row>
@@ -4504,7 +4515,7 @@
         <v>33.700000000000003</v>
       </c>
       <c r="E131" s="4">
-        <f>B131+C131/60+D131/3600</f>
+        <f t="shared" si="17"/>
         <v>31.676027777777779</v>
       </c>
       <c r="F131" s="1">
@@ -4517,7 +4528,7 @@
         <v>5.2</v>
       </c>
       <c r="I131">
-        <f>-F131-G131/60-H131/3600</f>
+        <f t="shared" si="16"/>
         <v>-91.834777777777774</v>
       </c>
     </row>
@@ -4535,7 +4546,7 @@
         <v>34.4</v>
       </c>
       <c r="E132" s="4">
-        <f>B132+C132/60+D132/3600</f>
+        <f t="shared" si="17"/>
         <v>31.609555555555556</v>
       </c>
       <c r="F132" s="1">
@@ -4548,7 +4559,7 @@
         <v>29.3</v>
       </c>
       <c r="I132">
-        <f>-F132-G132/60-H132/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.02480555555556</v>
       </c>
     </row>
@@ -4566,7 +4577,7 @@
         <v>22.367999999999999</v>
       </c>
       <c r="E133" s="4">
-        <f>B133+C133/60+D133/3600</f>
+        <f t="shared" si="17"/>
         <v>31.572880000000001</v>
       </c>
       <c r="F133" s="1">
@@ -4579,7 +4590,7 @@
         <v>23.7</v>
       </c>
       <c r="I133">
-        <f>-F133-G133/60-H133/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.023250000000004</v>
       </c>
     </row>
@@ -4597,7 +4608,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E134" s="4">
-        <f>B134+C134/60+D134/3600</f>
+        <f t="shared" si="17"/>
         <v>31.30113888888889</v>
       </c>
       <c r="F134" s="1">
@@ -4610,7 +4621,7 @@
         <v>24.9</v>
       </c>
       <c r="I134">
-        <f>-F134-G134/60-H134/3600</f>
+        <f t="shared" si="16"/>
         <v>-92.156916666666675</v>
       </c>
     </row>
@@ -4628,7 +4639,7 @@
         <v>15.49</v>
       </c>
       <c r="E135" s="4">
-        <f t="shared" ref="E133:E144" si="16">B135+C135/60+D135/3600</f>
+        <f t="shared" ref="E135:E144" si="18">B135+C135/60+D135/3600</f>
         <v>30.370969444444444</v>
       </c>
       <c r="F135" s="1">
@@ -4641,7 +4652,7 @@
         <v>31.54</v>
       </c>
       <c r="I135">
-        <f t="shared" ref="I133:I144" si="17">-F135-G135/60-H135/3600</f>
+        <f t="shared" ref="I135:I144" si="19">-F135-G135/60-H135/3600</f>
         <v>-91.625427777777773</v>
       </c>
     </row>
@@ -4659,7 +4670,7 @@
         <v>24.01</v>
       </c>
       <c r="E136" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.406669444444443</v>
       </c>
       <c r="F136" s="1">
@@ -4672,7 +4683,7 @@
         <v>31.88</v>
       </c>
       <c r="I136">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-91.692188888888893</v>
       </c>
     </row>
@@ -4690,7 +4701,7 @@
         <v>32.6</v>
       </c>
       <c r="E137" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.309055555555556</v>
       </c>
       <c r="F137" s="1">
@@ -4703,7 +4714,7 @@
         <v>17.2</v>
       </c>
       <c r="I137">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-91.771444444444441</v>
       </c>
     </row>
@@ -4721,7 +4732,7 @@
         <v>5.4</v>
       </c>
       <c r="E138" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.334833333333332</v>
       </c>
       <c r="F138" s="1">
@@ -4734,7 +4745,7 @@
         <v>39.6</v>
       </c>
       <c r="I138">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-90.044333333333327</v>
       </c>
     </row>
@@ -4752,7 +4763,7 @@
         <v>44.04</v>
       </c>
       <c r="E139" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.378900000000002</v>
       </c>
       <c r="F139" s="1">
@@ -4765,7 +4776,7 @@
         <v>39.491999999999997</v>
       </c>
       <c r="I139">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-90.160970000000006</v>
       </c>
     </row>
@@ -4783,7 +4794,7 @@
         <v>15.504</v>
       </c>
       <c r="E140" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.33764</v>
       </c>
       <c r="F140" s="1">
@@ -4796,7 +4807,7 @@
         <v>14.939</v>
       </c>
       <c r="I140">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-90.004149722222223</v>
       </c>
     </row>
@@ -4814,7 +4825,7 @@
         <v>5.7960000000000003</v>
       </c>
       <c r="E141" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.30161</v>
       </c>
       <c r="F141" s="1">
@@ -4827,7 +4838,7 @@
         <v>53.146999999999998</v>
       </c>
       <c r="I141">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-89.831429722222225</v>
       </c>
     </row>
@@ -4845,7 +4856,7 @@
         <v>56.195999999999998</v>
       </c>
       <c r="E142" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.165609999999997</v>
       </c>
       <c r="F142" s="1">
@@ -4858,7 +4869,7 @@
         <v>14.712</v>
       </c>
       <c r="I142">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-89.73742</v>
       </c>
     </row>
@@ -4876,7 +4887,7 @@
         <v>20.364000000000001</v>
       </c>
       <c r="E143" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.488990000000001</v>
       </c>
       <c r="F143" s="1">
@@ -4889,7 +4900,7 @@
         <v>41.064</v>
       </c>
       <c r="I143">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-90.094740000000002</v>
       </c>
     </row>
@@ -4907,7 +4918,7 @@
         <v>23.3</v>
       </c>
       <c r="E144" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>30.539805555555557</v>
       </c>
       <c r="F144" s="1">
@@ -4920,7 +4931,7 @@
         <v>28.2</v>
       </c>
       <c r="I144">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-89.874499999999998</v>
       </c>
     </row>
@@ -5957,9 +5968,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
   <dimension ref="A1:U144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G144" sqref="G144"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7150,7 +7161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12947,6 +12958,51 @@
       <c r="D120">
         <v>-93.512332999999998</v>
       </c>
+      <c r="E120" s="9">
+        <v>5</v>
+      </c>
+      <c r="F120" s="9">
+        <v>0</v>
+      </c>
+      <c r="G120" s="9">
+        <v>0</v>
+      </c>
+      <c r="H120" s="9">
+        <v>0</v>
+      </c>
+      <c r="I120" s="9">
+        <v>0</v>
+      </c>
+      <c r="J120" s="9">
+        <v>0</v>
+      </c>
+      <c r="K120" s="9">
+        <v>0</v>
+      </c>
+      <c r="L120" s="16">
+        <v>2</v>
+      </c>
+      <c r="M120" s="9">
+        <v>0</v>
+      </c>
+      <c r="N120" s="9">
+        <v>0</v>
+      </c>
+      <c r="O120" s="9">
+        <v>0</v>
+      </c>
+      <c r="P120" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="9">
+        <v>0</v>
+      </c>
+      <c r="R120" s="9">
+        <v>0</v>
+      </c>
+      <c r="S120" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A121">
@@ -12961,6 +13017,51 @@
       <c r="D121">
         <v>-93.741</v>
       </c>
+      <c r="E121" s="9">
+        <v>0</v>
+      </c>
+      <c r="F121" s="9">
+        <v>0</v>
+      </c>
+      <c r="G121" s="9">
+        <v>0</v>
+      </c>
+      <c r="H121" s="9">
+        <v>0</v>
+      </c>
+      <c r="I121" s="9">
+        <v>0</v>
+      </c>
+      <c r="J121" s="9">
+        <v>0</v>
+      </c>
+      <c r="K121" s="9">
+        <v>0</v>
+      </c>
+      <c r="L121" s="9">
+        <v>0</v>
+      </c>
+      <c r="M121" s="9">
+        <v>0</v>
+      </c>
+      <c r="N121" s="9">
+        <v>0</v>
+      </c>
+      <c r="O121" s="9">
+        <v>0</v>
+      </c>
+      <c r="P121" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="9">
+        <v>0</v>
+      </c>
+      <c r="R121" s="9">
+        <v>0</v>
+      </c>
+      <c r="S121" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A122">
@@ -12975,6 +13076,48 @@
       <c r="D122">
         <v>-93.850389000000007</v>
       </c>
+      <c r="E122" s="9">
+        <v>0</v>
+      </c>
+      <c r="F122" s="9">
+        <v>0</v>
+      </c>
+      <c r="G122" s="9">
+        <v>0</v>
+      </c>
+      <c r="H122" s="9">
+        <v>0</v>
+      </c>
+      <c r="I122" s="9">
+        <v>0</v>
+      </c>
+      <c r="J122" s="9">
+        <v>0</v>
+      </c>
+      <c r="K122" s="9">
+        <v>0</v>
+      </c>
+      <c r="L122" s="16">
+        <v>6</v>
+      </c>
+      <c r="M122" s="9">
+        <v>0</v>
+      </c>
+      <c r="N122" s="9">
+        <v>0</v>
+      </c>
+      <c r="O122" s="9">
+        <v>0</v>
+      </c>
+      <c r="P122" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q122" s="9">
+        <v>0</v>
+      </c>
+      <c r="R122" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A123">
@@ -12989,6 +13132,51 @@
       <c r="D123">
         <v>-92.641889000000006</v>
       </c>
+      <c r="E123" s="9">
+        <v>0</v>
+      </c>
+      <c r="F123" s="9">
+        <v>0</v>
+      </c>
+      <c r="G123" s="9">
+        <v>0</v>
+      </c>
+      <c r="H123" s="9">
+        <v>0</v>
+      </c>
+      <c r="I123" s="9">
+        <v>0</v>
+      </c>
+      <c r="J123" s="9">
+        <v>0</v>
+      </c>
+      <c r="K123" s="9">
+        <v>0</v>
+      </c>
+      <c r="L123" s="9">
+        <v>0</v>
+      </c>
+      <c r="M123" s="9">
+        <v>0</v>
+      </c>
+      <c r="N123" s="9">
+        <v>0</v>
+      </c>
+      <c r="O123" s="9">
+        <v>0</v>
+      </c>
+      <c r="P123" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q123" s="9">
+        <v>0</v>
+      </c>
+      <c r="R123" s="9">
+        <v>0</v>
+      </c>
+      <c r="S123" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A124">
@@ -13003,6 +13191,51 @@
       <c r="D124">
         <v>-92.649861000000001</v>
       </c>
+      <c r="E124" s="9">
+        <v>0</v>
+      </c>
+      <c r="F124" s="9">
+        <v>0</v>
+      </c>
+      <c r="G124" s="9">
+        <v>0</v>
+      </c>
+      <c r="H124" s="9">
+        <v>0</v>
+      </c>
+      <c r="I124" s="9">
+        <v>0</v>
+      </c>
+      <c r="J124" s="9">
+        <v>0</v>
+      </c>
+      <c r="K124" s="9">
+        <v>0</v>
+      </c>
+      <c r="L124" s="9">
+        <v>0</v>
+      </c>
+      <c r="M124" s="9">
+        <v>0</v>
+      </c>
+      <c r="N124" s="9">
+        <v>0</v>
+      </c>
+      <c r="O124" s="9">
+        <v>0</v>
+      </c>
+      <c r="P124" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="9">
+        <v>0</v>
+      </c>
+      <c r="R124" s="9">
+        <v>0</v>
+      </c>
+      <c r="S124" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A125">
@@ -13017,6 +13250,51 @@
       <c r="D125">
         <v>-92.575610999999995</v>
       </c>
+      <c r="E125" s="9">
+        <v>0</v>
+      </c>
+      <c r="F125" s="9">
+        <v>0</v>
+      </c>
+      <c r="G125" s="16">
+        <v>2</v>
+      </c>
+      <c r="H125" s="9">
+        <v>0</v>
+      </c>
+      <c r="I125" s="9">
+        <v>0</v>
+      </c>
+      <c r="J125" s="9">
+        <v>0</v>
+      </c>
+      <c r="K125" s="9">
+        <v>0</v>
+      </c>
+      <c r="L125" s="9">
+        <v>0</v>
+      </c>
+      <c r="M125" s="9">
+        <v>0</v>
+      </c>
+      <c r="N125" s="9">
+        <v>0</v>
+      </c>
+      <c r="O125" s="9">
+        <v>0</v>
+      </c>
+      <c r="P125" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q125" s="9">
+        <v>0</v>
+      </c>
+      <c r="R125" s="9">
+        <v>0</v>
+      </c>
+      <c r="S125" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A126">
@@ -13031,6 +13309,51 @@
       <c r="D126">
         <v>-92.490806000000006</v>
       </c>
+      <c r="E126" s="9">
+        <v>0</v>
+      </c>
+      <c r="F126" s="16">
+        <v>1</v>
+      </c>
+      <c r="G126" s="16">
+        <v>3</v>
+      </c>
+      <c r="H126" s="9">
+        <v>0</v>
+      </c>
+      <c r="I126" s="9">
+        <v>0</v>
+      </c>
+      <c r="J126" s="9">
+        <v>0</v>
+      </c>
+      <c r="K126" s="9">
+        <v>0</v>
+      </c>
+      <c r="L126" s="16">
+        <v>8</v>
+      </c>
+      <c r="M126" s="9">
+        <v>0</v>
+      </c>
+      <c r="N126" s="9">
+        <v>0</v>
+      </c>
+      <c r="O126" s="16">
+        <v>1</v>
+      </c>
+      <c r="P126" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="9">
+        <v>0</v>
+      </c>
+      <c r="R126" s="9">
+        <v>0</v>
+      </c>
+      <c r="S126" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A127">
@@ -13045,6 +13368,51 @@
       <c r="D127">
         <v>-91.766943999999995</v>
       </c>
+      <c r="E127" s="16">
+        <v>3</v>
+      </c>
+      <c r="F127" s="9">
+        <v>0</v>
+      </c>
+      <c r="G127" s="9">
+        <v>0</v>
+      </c>
+      <c r="H127" s="9">
+        <v>0</v>
+      </c>
+      <c r="I127" s="9">
+        <v>0</v>
+      </c>
+      <c r="J127" s="9">
+        <v>0</v>
+      </c>
+      <c r="K127" s="9">
+        <v>0</v>
+      </c>
+      <c r="L127" s="16">
+        <v>2</v>
+      </c>
+      <c r="M127" s="9">
+        <v>0</v>
+      </c>
+      <c r="N127" s="9">
+        <v>0</v>
+      </c>
+      <c r="O127" s="9">
+        <v>0</v>
+      </c>
+      <c r="P127" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q127" s="9">
+        <v>0</v>
+      </c>
+      <c r="R127" s="9">
+        <v>0</v>
+      </c>
+      <c r="S127" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A128">
@@ -13059,8 +13427,53 @@
       <c r="D128">
         <v>-91.192222000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128" s="9">
+        <v>0</v>
+      </c>
+      <c r="F128" s="9">
+        <v>0</v>
+      </c>
+      <c r="G128" s="9">
+        <v>0</v>
+      </c>
+      <c r="H128" s="9">
+        <v>0</v>
+      </c>
+      <c r="I128" s="9">
+        <v>0</v>
+      </c>
+      <c r="J128" s="9">
+        <v>0</v>
+      </c>
+      <c r="K128" s="9">
+        <v>0</v>
+      </c>
+      <c r="L128" s="16">
+        <v>2</v>
+      </c>
+      <c r="M128" s="9">
+        <v>0</v>
+      </c>
+      <c r="N128" s="9">
+        <v>0</v>
+      </c>
+      <c r="O128" s="9">
+        <v>0</v>
+      </c>
+      <c r="P128" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="9">
+        <v>0</v>
+      </c>
+      <c r="R128" s="9">
+        <v>0</v>
+      </c>
+      <c r="S128" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>126</v>
       </c>
@@ -13073,8 +13486,53 @@
       <c r="D129">
         <v>-91.834778</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129" s="9">
+        <v>0</v>
+      </c>
+      <c r="F129" s="9">
+        <v>0</v>
+      </c>
+      <c r="G129" s="9">
+        <v>0</v>
+      </c>
+      <c r="H129" s="9">
+        <v>0</v>
+      </c>
+      <c r="I129" s="9">
+        <v>0</v>
+      </c>
+      <c r="J129" s="9">
+        <v>0</v>
+      </c>
+      <c r="K129" s="9">
+        <v>0</v>
+      </c>
+      <c r="L129" s="16">
+        <v>8</v>
+      </c>
+      <c r="M129" s="9">
+        <v>0</v>
+      </c>
+      <c r="N129" s="9">
+        <v>0</v>
+      </c>
+      <c r="O129" s="9">
+        <v>0</v>
+      </c>
+      <c r="P129" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="9">
+        <v>0</v>
+      </c>
+      <c r="R129" s="9">
+        <v>0</v>
+      </c>
+      <c r="S129" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>127</v>
       </c>
@@ -13087,12 +13545,57 @@
       <c r="D130">
         <v>-92.024805999999998</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130" s="9">
+        <v>0</v>
+      </c>
+      <c r="F130" s="9">
+        <v>0</v>
+      </c>
+      <c r="G130" s="9">
+        <v>0</v>
+      </c>
+      <c r="H130" s="9">
+        <v>0</v>
+      </c>
+      <c r="I130" s="9">
+        <v>0</v>
+      </c>
+      <c r="J130" s="9">
+        <v>0</v>
+      </c>
+      <c r="K130" s="9">
+        <v>0</v>
+      </c>
+      <c r="L130" s="9">
+        <v>0</v>
+      </c>
+      <c r="M130" s="9">
+        <v>0</v>
+      </c>
+      <c r="N130" s="9">
+        <v>0</v>
+      </c>
+      <c r="O130" s="9">
+        <v>0</v>
+      </c>
+      <c r="P130" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="9">
+        <v>0</v>
+      </c>
+      <c r="R130" s="9">
+        <v>0</v>
+      </c>
+      <c r="S130" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>128</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C131">
@@ -13101,8 +13604,53 @@
       <c r="D131">
         <v>-92.023250000000004</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E131" s="9">
+        <v>0</v>
+      </c>
+      <c r="F131" s="9">
+        <v>0</v>
+      </c>
+      <c r="G131" s="9">
+        <v>0</v>
+      </c>
+      <c r="H131" s="9">
+        <v>0</v>
+      </c>
+      <c r="I131" s="9">
+        <v>0</v>
+      </c>
+      <c r="J131" s="9">
+        <v>0</v>
+      </c>
+      <c r="K131" s="9">
+        <v>0</v>
+      </c>
+      <c r="L131" s="16">
+        <v>1</v>
+      </c>
+      <c r="M131" s="9">
+        <v>0</v>
+      </c>
+      <c r="N131" s="9">
+        <v>0</v>
+      </c>
+      <c r="O131" s="9">
+        <v>0</v>
+      </c>
+      <c r="P131" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="9">
+        <v>0</v>
+      </c>
+      <c r="R131" s="9">
+        <v>0</v>
+      </c>
+      <c r="S131" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>129</v>
       </c>
@@ -13115,8 +13663,53 @@
       <c r="D132">
         <v>-92.156917000000007</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132" s="9">
+        <v>0</v>
+      </c>
+      <c r="F132" s="9">
+        <v>0</v>
+      </c>
+      <c r="G132" s="16">
+        <v>7</v>
+      </c>
+      <c r="H132" s="9">
+        <v>0</v>
+      </c>
+      <c r="I132" s="9">
+        <v>0</v>
+      </c>
+      <c r="J132" s="9">
+        <v>0</v>
+      </c>
+      <c r="K132" s="9">
+        <v>0</v>
+      </c>
+      <c r="L132" s="14">
+        <v>0</v>
+      </c>
+      <c r="M132" s="9">
+        <v>0</v>
+      </c>
+      <c r="N132" s="9">
+        <v>0</v>
+      </c>
+      <c r="O132" s="16">
+        <v>1</v>
+      </c>
+      <c r="P132" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q132" s="9">
+        <v>0</v>
+      </c>
+      <c r="R132" s="9">
+        <v>0</v>
+      </c>
+      <c r="S132" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>130</v>
       </c>
@@ -13129,8 +13722,53 @@
       <c r="D133">
         <v>-91.625427999999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E133" s="9">
+        <v>0</v>
+      </c>
+      <c r="F133" s="9">
+        <v>0</v>
+      </c>
+      <c r="G133" s="9">
+        <v>0</v>
+      </c>
+      <c r="H133" s="9">
+        <v>0</v>
+      </c>
+      <c r="I133" s="9">
+        <v>0</v>
+      </c>
+      <c r="J133" s="9">
+        <v>0</v>
+      </c>
+      <c r="K133" s="9">
+        <v>0</v>
+      </c>
+      <c r="L133" s="9">
+        <v>0</v>
+      </c>
+      <c r="M133" s="9">
+        <v>0</v>
+      </c>
+      <c r="N133" s="9">
+        <v>0</v>
+      </c>
+      <c r="O133" s="9">
+        <v>0</v>
+      </c>
+      <c r="P133" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q133" s="9">
+        <v>0</v>
+      </c>
+      <c r="R133" s="9">
+        <v>0</v>
+      </c>
+      <c r="S133" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>131</v>
       </c>
@@ -13143,8 +13781,53 @@
       <c r="D134">
         <v>-91.692188999999999</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E134" s="16">
+        <v>1</v>
+      </c>
+      <c r="F134" s="9">
+        <v>0</v>
+      </c>
+      <c r="G134" s="9">
+        <v>0</v>
+      </c>
+      <c r="H134" s="9">
+        <v>0</v>
+      </c>
+      <c r="I134" s="9">
+        <v>0</v>
+      </c>
+      <c r="J134" s="9">
+        <v>0</v>
+      </c>
+      <c r="K134" s="9">
+        <v>0</v>
+      </c>
+      <c r="L134" s="9">
+        <v>0</v>
+      </c>
+      <c r="M134" s="9">
+        <v>0</v>
+      </c>
+      <c r="N134" s="9">
+        <v>0</v>
+      </c>
+      <c r="O134" s="9">
+        <v>0</v>
+      </c>
+      <c r="P134" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="9">
+        <v>0</v>
+      </c>
+      <c r="R134" s="9">
+        <v>0</v>
+      </c>
+      <c r="S134" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>132</v>
       </c>
@@ -13157,8 +13840,54 @@
       <c r="D135">
         <v>-91.771444000000002</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E135" s="16">
+        <v>9</v>
+      </c>
+      <c r="F135" s="18">
+        <v>0</v>
+      </c>
+      <c r="G135" s="18">
+        <v>0</v>
+      </c>
+      <c r="H135" s="18">
+        <v>0</v>
+      </c>
+      <c r="I135" s="18">
+        <v>0</v>
+      </c>
+      <c r="J135" s="18">
+        <v>0</v>
+      </c>
+      <c r="K135" s="18">
+        <v>0</v>
+      </c>
+      <c r="L135" s="18">
+        <v>0</v>
+      </c>
+      <c r="M135" s="18">
+        <v>0</v>
+      </c>
+      <c r="N135" s="18">
+        <v>0</v>
+      </c>
+      <c r="O135" s="18">
+        <v>0</v>
+      </c>
+      <c r="P135" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="18">
+        <v>0</v>
+      </c>
+      <c r="R135" s="18">
+        <v>0</v>
+      </c>
+      <c r="S135" s="18">
+        <v>0</v>
+      </c>
+      <c r="T135" s="18"/>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>133</v>
       </c>
@@ -13171,8 +13900,53 @@
       <c r="D136">
         <v>-90.044332999999995</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136" s="18">
+        <v>0</v>
+      </c>
+      <c r="F136" s="18">
+        <v>0</v>
+      </c>
+      <c r="G136" s="19">
+        <v>5</v>
+      </c>
+      <c r="H136" s="18">
+        <v>0</v>
+      </c>
+      <c r="I136" s="18">
+        <v>0</v>
+      </c>
+      <c r="J136" s="18">
+        <v>0</v>
+      </c>
+      <c r="K136" s="18">
+        <v>0</v>
+      </c>
+      <c r="L136" s="18">
+        <v>0</v>
+      </c>
+      <c r="M136" s="18">
+        <v>0</v>
+      </c>
+      <c r="N136" s="18">
+        <v>0</v>
+      </c>
+      <c r="O136" s="18">
+        <v>0</v>
+      </c>
+      <c r="P136" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q136" s="18">
+        <v>0</v>
+      </c>
+      <c r="R136" s="18">
+        <v>0</v>
+      </c>
+      <c r="S136" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>134</v>
       </c>
@@ -13185,8 +13959,53 @@
       <c r="D137">
         <v>-90.160970000000006</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137" s="18">
+        <v>0</v>
+      </c>
+      <c r="F137" s="18">
+        <v>0</v>
+      </c>
+      <c r="G137" s="19">
+        <v>7</v>
+      </c>
+      <c r="H137" s="18">
+        <v>0</v>
+      </c>
+      <c r="I137" s="18">
+        <v>0</v>
+      </c>
+      <c r="J137" s="18">
+        <v>0</v>
+      </c>
+      <c r="K137" s="18">
+        <v>0</v>
+      </c>
+      <c r="L137" s="18">
+        <v>0</v>
+      </c>
+      <c r="M137" s="18">
+        <v>0</v>
+      </c>
+      <c r="N137" s="18">
+        <v>0</v>
+      </c>
+      <c r="O137" s="18">
+        <v>0</v>
+      </c>
+      <c r="P137" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="18">
+        <v>0</v>
+      </c>
+      <c r="R137" s="18">
+        <v>0</v>
+      </c>
+      <c r="S137" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>135</v>
       </c>
@@ -13199,8 +14018,53 @@
       <c r="D138">
         <v>-90.004149999999996</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138" s="9">
+        <v>0</v>
+      </c>
+      <c r="F138" s="9">
+        <v>0</v>
+      </c>
+      <c r="G138" s="9">
+        <v>0</v>
+      </c>
+      <c r="H138" s="9">
+        <v>0</v>
+      </c>
+      <c r="I138" s="9">
+        <v>0</v>
+      </c>
+      <c r="J138" s="9">
+        <v>0</v>
+      </c>
+      <c r="K138" s="9">
+        <v>0</v>
+      </c>
+      <c r="L138" s="9">
+        <v>0</v>
+      </c>
+      <c r="M138" s="9">
+        <v>0</v>
+      </c>
+      <c r="N138" s="9">
+        <v>0</v>
+      </c>
+      <c r="O138" s="9">
+        <v>0</v>
+      </c>
+      <c r="P138" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="9">
+        <v>0</v>
+      </c>
+      <c r="R138" s="9">
+        <v>0</v>
+      </c>
+      <c r="S138" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>136</v>
       </c>
@@ -13213,8 +14077,53 @@
       <c r="D139">
         <v>-89.831429999999997</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E139" s="9">
+        <v>0</v>
+      </c>
+      <c r="F139" s="9">
+        <v>0</v>
+      </c>
+      <c r="G139" s="9">
+        <v>0</v>
+      </c>
+      <c r="H139" s="9">
+        <v>0</v>
+      </c>
+      <c r="I139" s="9">
+        <v>0</v>
+      </c>
+      <c r="J139" s="9">
+        <v>0</v>
+      </c>
+      <c r="K139" s="9">
+        <v>0</v>
+      </c>
+      <c r="L139" s="9">
+        <v>0</v>
+      </c>
+      <c r="M139" s="9">
+        <v>0</v>
+      </c>
+      <c r="N139" s="9">
+        <v>0</v>
+      </c>
+      <c r="O139" s="9">
+        <v>0</v>
+      </c>
+      <c r="P139" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="9">
+        <v>0</v>
+      </c>
+      <c r="R139" s="9">
+        <v>0</v>
+      </c>
+      <c r="S139" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>137</v>
       </c>
@@ -13227,8 +14136,53 @@
       <c r="D140">
         <v>-89.73742</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140" s="9">
+        <v>0</v>
+      </c>
+      <c r="F140" s="9">
+        <v>0</v>
+      </c>
+      <c r="G140" s="9">
+        <v>0</v>
+      </c>
+      <c r="H140" s="9">
+        <v>0</v>
+      </c>
+      <c r="I140" s="9">
+        <v>0</v>
+      </c>
+      <c r="J140" s="9">
+        <v>0</v>
+      </c>
+      <c r="K140" s="9">
+        <v>0</v>
+      </c>
+      <c r="L140" s="9">
+        <v>0</v>
+      </c>
+      <c r="M140" s="9">
+        <v>0</v>
+      </c>
+      <c r="N140" s="9">
+        <v>0</v>
+      </c>
+      <c r="O140" s="9">
+        <v>0</v>
+      </c>
+      <c r="P140" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="9">
+        <v>0</v>
+      </c>
+      <c r="R140" s="9">
+        <v>0</v>
+      </c>
+      <c r="S140" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>138</v>
       </c>
@@ -13241,8 +14195,53 @@
       <c r="D141">
         <v>-90.094740000000002</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141" s="9">
+        <v>0</v>
+      </c>
+      <c r="F141" s="9">
+        <v>0</v>
+      </c>
+      <c r="G141" s="9">
+        <v>0</v>
+      </c>
+      <c r="H141" s="9">
+        <v>0</v>
+      </c>
+      <c r="I141" s="9">
+        <v>0</v>
+      </c>
+      <c r="J141" s="9">
+        <v>0</v>
+      </c>
+      <c r="K141" s="9">
+        <v>0</v>
+      </c>
+      <c r="L141" s="9">
+        <v>0</v>
+      </c>
+      <c r="M141" s="9">
+        <v>0</v>
+      </c>
+      <c r="N141" s="9">
+        <v>0</v>
+      </c>
+      <c r="O141" s="9">
+        <v>0</v>
+      </c>
+      <c r="P141" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q141" s="9">
+        <v>0</v>
+      </c>
+      <c r="R141" s="9">
+        <v>0</v>
+      </c>
+      <c r="S141" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>139</v>
       </c>
@@ -13255,8 +14254,112 @@
       <c r="D142">
         <v>-89.874499999999998</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E142" s="18">
+        <v>0</v>
+      </c>
+      <c r="F142" s="18">
+        <v>0</v>
+      </c>
+      <c r="G142" s="18">
+        <v>0</v>
+      </c>
+      <c r="H142" s="18">
+        <v>0</v>
+      </c>
+      <c r="I142" s="18">
+        <v>0</v>
+      </c>
+      <c r="J142" s="18">
+        <v>0</v>
+      </c>
+      <c r="K142" s="19">
+        <v>5</v>
+      </c>
+      <c r="L142" s="18">
+        <v>0</v>
+      </c>
+      <c r="M142" s="18">
+        <v>0</v>
+      </c>
+      <c r="N142" s="18">
+        <v>0</v>
+      </c>
+      <c r="O142" s="18">
+        <v>0</v>
+      </c>
+      <c r="P142" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q142" s="18">
+        <v>0</v>
+      </c>
+      <c r="R142" s="18">
+        <v>0</v>
+      </c>
+      <c r="S142" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>140</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143">
+        <v>30.869166400000001</v>
+      </c>
+      <c r="D143">
+        <v>-91.303483888888806</v>
+      </c>
+      <c r="E143" s="9">
+        <v>0</v>
+      </c>
+      <c r="F143" s="9">
+        <v>0</v>
+      </c>
+      <c r="G143" s="9">
+        <v>0</v>
+      </c>
+      <c r="H143" s="9">
+        <v>0</v>
+      </c>
+      <c r="I143" s="9">
+        <v>0</v>
+      </c>
+      <c r="J143" s="9">
+        <v>0</v>
+      </c>
+      <c r="K143" s="9">
+        <v>0</v>
+      </c>
+      <c r="L143" s="9">
+        <v>0</v>
+      </c>
+      <c r="M143" s="9">
+        <v>0</v>
+      </c>
+      <c r="N143" s="9">
+        <v>0</v>
+      </c>
+      <c r="O143" s="9">
+        <v>0</v>
+      </c>
+      <c r="P143" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q143" s="9">
+        <v>0</v>
+      </c>
+      <c r="R143" s="9">
+        <v>0</v>
+      </c>
+      <c r="S143" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D144" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed R. cerebellata map.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimehrotra/Desktop/spongehunters/map_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAF5E87-7F4B-EB4D-BA32-CA4337119B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A01E20-571F-3043-87E3-6D98D9F27623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="7" xr2:uid="{EBB5A95D-9C71-6541-A106-6E906091C46C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate GPS Coordinates" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="27">
   <si>
     <t>Long</t>
   </si>
@@ -7137,9 +7137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A34F3-001A-814F-9795-6302158BAD39}">
   <dimension ref="A1:U173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A146" sqref="A146:D146"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12017,7 +12017,7 @@
         <v>0</v>
       </c>
       <c r="J83" s="12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K83" s="10">
         <v>0</v>
@@ -17628,8 +17628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60BEF1D-CE3F-0443-9C24-2B53E5F8D838}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17666,18 +17666,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>83</v>
-      </c>
-      <c r="B3">
-        <v>29.987055555555557</v>
-      </c>
-      <c r="C3">
-        <v>-90.091555555555544</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3"/>
+      <c r="C3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated some of the maps.
</commit_message>
<xml_diff>
--- a/map_data_files/GPS Coordinates - Sites and Species.xlsx
+++ b/map_data_files/GPS Coordinates - Sites and Species.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spongehunters\map_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="27">
   <si>
     <t>Long</t>
   </si>
@@ -579,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L183"/>
+  <dimension ref="A1:L184"/>
   <sheetViews>
     <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+      <selection activeCell="I184" sqref="I184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4647,7 +4647,7 @@
         <v>15.49</v>
       </c>
       <c r="E135" s="4">
-        <f t="shared" ref="E135:E183" si="18">B135+C135/60+D135/3600</f>
+        <f t="shared" ref="E135:E184" si="18">B135+C135/60+D135/3600</f>
         <v>30.370969444444444</v>
       </c>
       <c r="F135" s="1">
@@ -4660,7 +4660,7 @@
         <v>31.54</v>
       </c>
       <c r="I135">
-        <f t="shared" ref="I135:I183" si="19">-F135-G135/60-H135/3600</f>
+        <f t="shared" ref="I135:I184" si="19">-F135-G135/60-H135/3600</f>
         <v>-91.625427777777773</v>
       </c>
     </row>
@@ -6150,6 +6150,37 @@
       <c r="I183">
         <f t="shared" si="19"/>
         <v>-91.512002222222222</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9">
+      <c r="A184">
+        <v>179</v>
+      </c>
+      <c r="B184" s="1">
+        <v>30</v>
+      </c>
+      <c r="C184">
+        <v>34</v>
+      </c>
+      <c r="D184">
+        <v>8.9760000000000009</v>
+      </c>
+      <c r="E184" s="4">
+        <f t="shared" si="18"/>
+        <v>30.56916</v>
+      </c>
+      <c r="F184" s="1">
+        <v>91</v>
+      </c>
+      <c r="G184">
+        <v>9</v>
+      </c>
+      <c r="H184">
+        <v>57.887</v>
+      </c>
+      <c r="I184">
+        <f t="shared" si="19"/>
+        <v>-91.166079722222221</v>
       </c>
     </row>
   </sheetData>
@@ -6811,10 +6842,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6838,13 +6869,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B2">
-        <v>30.126750000000001</v>
+        <v>29.987055555555557</v>
       </c>
       <c r="C2">
-        <v>-91.27847222222222</v>
+        <v>-90.091555555555544</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -6852,13 +6883,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3">
-        <v>29.987055555555557</v>
+        <v>30.00375</v>
       </c>
       <c r="C3">
-        <v>-90.091555555555544</v>
+        <v>-90.096166666666662</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -6866,13 +6897,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4">
-        <v>30.00375</v>
+        <v>29.983249999999998</v>
       </c>
       <c r="C4">
-        <v>-90.096166666666662</v>
+        <v>-90.090305555555545</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>3</v>
@@ -6880,13 +6911,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B5">
-        <v>29.983249999999998</v>
+        <v>30.02547222222222</v>
       </c>
       <c r="C5">
-        <v>-90.090305555555545</v>
+        <v>-90.115638888888881</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -6894,13 +6925,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="B6">
-        <v>30.02547222222222</v>
-      </c>
-      <c r="C6">
-        <v>-90.115638888888881</v>
+        <v>30.0215</v>
+      </c>
+      <c r="C6" s="4">
+        <v>-90.15313888888889</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>3</v>
@@ -6908,13 +6939,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B7">
-        <v>30.0215</v>
-      </c>
-      <c r="C7" s="4">
-        <v>-90.15313888888889</v>
+        <v>30.026527777777776</v>
+      </c>
+      <c r="C7">
+        <v>-90.08197222222222</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
@@ -6922,29 +6953,15 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B8">
-        <v>30.026527777777776</v>
+        <v>30.06527777777778</v>
       </c>
       <c r="C8">
-        <v>-90.08197222222222</v>
+        <v>-89.806527777777774</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>144</v>
-      </c>
-      <c r="B9">
-        <v>30.06527777777778</v>
-      </c>
-      <c r="C9">
-        <v>-89.806527777777774</v>
-      </c>
-      <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6955,10 +6972,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7021,13 +7038,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="B5">
-        <v>30.456499999999998</v>
+        <v>30.126750000000001</v>
       </c>
       <c r="C5">
-        <v>-89.784777777777776</v>
+        <v>-91.27847222222222</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -7035,15 +7052,29 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
+        <v>95</v>
+      </c>
+      <c r="B6">
+        <v>30.456499999999998</v>
+      </c>
+      <c r="C6">
+        <v>-89.784777777777776</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>96</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>30.49677777777778</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>-89.814472222222221</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7351,11 +7382,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U180"/>
+  <dimension ref="A1:U181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G179" sqref="G179"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G175" sqref="G175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -9351,10 +9382,10 @@
         <v>1</v>
       </c>
       <c r="M34" s="10">
+        <v>0</v>
+      </c>
+      <c r="N34" s="10">
         <v>2</v>
-      </c>
-      <c r="N34" s="10">
-        <v>0</v>
       </c>
       <c r="O34" s="10">
         <v>0</v>
@@ -16544,6 +16575,20 @@
       </c>
       <c r="D180">
         <v>-91.512002222222222</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181">
+        <v>179</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181">
+        <v>30.56916</v>
+      </c>
+      <c r="D181">
+        <v>-91.166079722222221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>